<commit_message>
Fixing serial connection bug
</commit_message>
<xml_diff>
--- a/dist/Hola.xlsx
+++ b/dist/Hola.xlsx
@@ -323,7 +323,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1238,7 +1238,7 @@
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>21-05-23 17:27:25</t>
+          <t>21-05-25 08:44:03</t>
         </is>
       </c>
       <c r="B65" s="0" t="n"/>
@@ -1249,7 +1249,7 @@
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>21-05-23 17:27:29</t>
+          <t>21-05-25 08:45:51</t>
         </is>
       </c>
       <c r="B66" s="0" t="n"/>
@@ -1260,7 +1260,7 @@
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>21-05-23 17:27:33</t>
+          <t>21-05-25 12:44:57</t>
         </is>
       </c>
       <c r="B67" s="0" t="n"/>
@@ -1271,7 +1271,7 @@
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>21-05-23 17:27:38</t>
+          <t>21-05-25 13:03:49</t>
         </is>
       </c>
       <c r="B68" s="0" t="n"/>
@@ -1282,7 +1282,7 @@
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>21-05-23 17:27:42</t>
+          <t>21-05-25 13:04:12</t>
         </is>
       </c>
       <c r="B69" s="0" t="n"/>
@@ -1293,7 +1293,7 @@
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>21-05-23 17:27:47</t>
+          <t>21-05-25 13:26:47</t>
         </is>
       </c>
       <c r="B70" s="0" t="n"/>
@@ -1302,575 +1302,21 @@
       <c r="E70" s="0" t="n"/>
     </row>
     <row r="71">
-      <c r="A71" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:27:51</t>
-        </is>
-      </c>
-      <c r="B71" s="0" t="n"/>
-      <c r="C71" s="0" t="n"/>
-      <c r="D71" s="0" t="n"/>
-      <c r="E71" s="0" t="n"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:27:56</t>
-        </is>
-      </c>
-      <c r="B72" s="0" t="n"/>
-      <c r="C72" s="0" t="n"/>
-      <c r="D72" s="0" t="n"/>
-      <c r="E72" s="0" t="n"/>
-    </row>
-    <row r="73">
-      <c r="A73" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:00</t>
-        </is>
-      </c>
-      <c r="B73" s="0" t="n"/>
-      <c r="C73" s="0" t="n"/>
-      <c r="D73" s="0" t="n"/>
-      <c r="E73" s="0" t="n"/>
-    </row>
-    <row r="74">
-      <c r="A74" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:05</t>
-        </is>
-      </c>
-      <c r="B74" s="0" t="n"/>
-      <c r="C74" s="0" t="n"/>
-      <c r="D74" s="0" t="n"/>
-      <c r="E74" s="0" t="n"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:08</t>
-        </is>
-      </c>
-      <c r="B75" s="0" t="n"/>
-      <c r="C75" s="0" t="n"/>
-      <c r="D75" s="0" t="n"/>
-      <c r="E75" s="0" t="n"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:11</t>
-        </is>
-      </c>
-      <c r="B76" s="0" t="n"/>
-      <c r="C76" s="0" t="n"/>
-      <c r="D76" s="0" t="n"/>
-      <c r="E76" s="0" t="n"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:13</t>
-        </is>
-      </c>
-      <c r="B77" s="0" t="n"/>
-      <c r="C77" s="0" t="n"/>
-      <c r="D77" s="0" t="n"/>
-      <c r="E77" s="0" t="n"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:16</t>
-        </is>
-      </c>
-      <c r="B78" s="0" t="n"/>
-      <c r="C78" s="0" t="n"/>
-      <c r="D78" s="0" t="n"/>
-      <c r="E78" s="0" t="n"/>
-    </row>
-    <row r="79">
-      <c r="A79" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:18</t>
-        </is>
-      </c>
-      <c r="B79" s="0" t="n"/>
-      <c r="C79" s="0" t="n"/>
-      <c r="D79" s="0" t="n"/>
-      <c r="E79" s="0" t="n"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:21</t>
-        </is>
-      </c>
-      <c r="B80" s="0" t="n"/>
-      <c r="C80" s="0" t="n"/>
-      <c r="D80" s="0" t="n"/>
-      <c r="E80" s="0" t="n"/>
-    </row>
-    <row r="81">
-      <c r="A81" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:23</t>
-        </is>
-      </c>
-      <c r="B81" s="0" t="n"/>
-      <c r="C81" s="0" t="n"/>
-      <c r="D81" s="0" t="n"/>
-      <c r="E81" s="0" t="n"/>
-    </row>
-    <row r="82">
-      <c r="A82" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:26</t>
-        </is>
-      </c>
-      <c r="B82" s="0" t="n"/>
-      <c r="C82" s="0" t="n"/>
-      <c r="D82" s="0" t="n"/>
-      <c r="E82" s="0" t="n"/>
-    </row>
-    <row r="83">
-      <c r="A83" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:28</t>
-        </is>
-      </c>
-      <c r="B83" s="0" t="n"/>
-      <c r="C83" s="0" t="n"/>
-      <c r="D83" s="0" t="n"/>
-      <c r="E83" s="0" t="n"/>
-    </row>
-    <row r="84">
-      <c r="A84" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:31</t>
-        </is>
-      </c>
-      <c r="B84" s="0" t="n"/>
-      <c r="C84" s="0" t="n"/>
-      <c r="D84" s="0" t="n"/>
-      <c r="E84" s="0" t="n"/>
-    </row>
-    <row r="85">
-      <c r="A85" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:33</t>
-        </is>
-      </c>
-      <c r="B85" s="0" t="n"/>
-      <c r="C85" s="0" t="n"/>
-      <c r="D85" s="0" t="n"/>
-      <c r="E85" s="0" t="n"/>
-    </row>
-    <row r="86">
-      <c r="A86" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:36</t>
-        </is>
-      </c>
-      <c r="B86" s="0" t="n"/>
-      <c r="C86" s="0" t="n"/>
-      <c r="D86" s="0" t="n"/>
-      <c r="E86" s="0" t="n"/>
-    </row>
-    <row r="87">
-      <c r="A87" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:38</t>
-        </is>
-      </c>
-      <c r="B87" s="0" t="n"/>
-      <c r="C87" s="0" t="n"/>
-      <c r="D87" s="0" t="n"/>
-      <c r="E87" s="0" t="n"/>
-    </row>
-    <row r="88">
-      <c r="A88" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:41</t>
-        </is>
-      </c>
-      <c r="B88" s="0" t="n"/>
-      <c r="C88" s="0" t="n"/>
-      <c r="D88" s="0" t="n"/>
-      <c r="E88" s="0" t="n"/>
-    </row>
-    <row r="89">
-      <c r="A89" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:43</t>
-        </is>
-      </c>
-      <c r="B89" s="0" t="n"/>
-      <c r="C89" s="0" t="n"/>
-      <c r="D89" s="0" t="n"/>
-      <c r="E89" s="0" t="n"/>
-    </row>
-    <row r="90">
-      <c r="A90" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:46</t>
-        </is>
-      </c>
-      <c r="B90" s="0" t="n"/>
-      <c r="C90" s="0" t="n"/>
-      <c r="D90" s="0" t="n"/>
-      <c r="E90" s="0" t="n"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="0" t="inlineStr">
-        <is>
-          <t>21-05-23 17:28:48</t>
-        </is>
-      </c>
-      <c r="B91" s="0" t="n"/>
-      <c r="C91" s="0" t="n"/>
-      <c r="D91" s="0" t="n"/>
-      <c r="E91" s="0" t="n"/>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>21-05-23 17:30:17</t>
-        </is>
-      </c>
-      <c r="B92" t="n">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>21-05-25 13:27:07</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
         <v/>
       </c>
-      <c r="C92" t="n">
+      <c r="C71" t="n">
         <v/>
       </c>
-      <c r="D92" t="n">
+      <c r="D71" t="n">
         <v/>
       </c>
-      <c r="E92" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>21-05-23 17:30:24</t>
-        </is>
-      </c>
-      <c r="B93" t="n">
-        <v/>
-      </c>
-      <c r="C93" t="n">
-        <v/>
-      </c>
-      <c r="D93" t="n">
-        <v/>
-      </c>
-      <c r="E93" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>21-05-23 17:30:29</t>
-        </is>
-      </c>
-      <c r="B94" t="n">
-        <v/>
-      </c>
-      <c r="C94" t="n">
-        <v/>
-      </c>
-      <c r="D94" t="n">
-        <v/>
-      </c>
-      <c r="E94" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>21-05-23 17:30:33</t>
-        </is>
-      </c>
-      <c r="B95" t="n">
-        <v/>
-      </c>
-      <c r="C95" t="n">
-        <v/>
-      </c>
-      <c r="D95" t="n">
-        <v/>
-      </c>
-      <c r="E95" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>21-05-23 17:30:36</t>
-        </is>
-      </c>
-      <c r="B96" t="n">
-        <v/>
-      </c>
-      <c r="C96" t="n">
-        <v/>
-      </c>
-      <c r="D96" t="n">
-        <v/>
-      </c>
-      <c r="E96" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>21-05-23 17:30:39</t>
-        </is>
-      </c>
-      <c r="B97" t="n">
-        <v/>
-      </c>
-      <c r="C97" t="n">
-        <v/>
-      </c>
-      <c r="D97" t="n">
-        <v/>
-      </c>
-      <c r="E97" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>21-05-23 17:30:41</t>
-        </is>
-      </c>
-      <c r="B98" t="n">
-        <v/>
-      </c>
-      <c r="C98" t="n">
-        <v/>
-      </c>
-      <c r="D98" t="n">
-        <v/>
-      </c>
-      <c r="E98" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>21-05-23 17:30:44</t>
-        </is>
-      </c>
-      <c r="B99" t="n">
-        <v/>
-      </c>
-      <c r="C99" t="n">
-        <v/>
-      </c>
-      <c r="D99" t="n">
-        <v/>
-      </c>
-      <c r="E99" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>21-05-23 17:31:03</t>
-        </is>
-      </c>
-      <c r="B100" t="n">
-        <v/>
-      </c>
-      <c r="C100" t="n">
-        <v/>
-      </c>
-      <c r="D100" t="n">
-        <v/>
-      </c>
-      <c r="E100" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>21-05-23 17:31:05</t>
-        </is>
-      </c>
-      <c r="B101" t="n">
-        <v/>
-      </c>
-      <c r="C101" t="n">
-        <v/>
-      </c>
-      <c r="D101" t="n">
-        <v/>
-      </c>
-      <c r="E101" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>21-05-23 17:31:08</t>
-        </is>
-      </c>
-      <c r="B102" t="n">
-        <v/>
-      </c>
-      <c r="C102" t="n">
-        <v/>
-      </c>
-      <c r="D102" t="n">
-        <v/>
-      </c>
-      <c r="E102" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>21-05-23 17:31:10</t>
-        </is>
-      </c>
-      <c r="B103" t="n">
-        <v/>
-      </c>
-      <c r="C103" t="n">
-        <v/>
-      </c>
-      <c r="D103" t="n">
-        <v/>
-      </c>
-      <c r="E103" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>21-05-23 17:31:13</t>
-        </is>
-      </c>
-      <c r="B104" t="n">
-        <v/>
-      </c>
-      <c r="C104" t="n">
-        <v/>
-      </c>
-      <c r="D104" t="n">
-        <v/>
-      </c>
-      <c r="E104" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>21-05-23 17:31:15</t>
-        </is>
-      </c>
-      <c r="B105" t="n">
-        <v/>
-      </c>
-      <c r="C105" t="n">
-        <v/>
-      </c>
-      <c r="D105" t="n">
-        <v/>
-      </c>
-      <c r="E105" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>21-05-23 17:31:18</t>
-        </is>
-      </c>
-      <c r="B106" t="n">
-        <v/>
-      </c>
-      <c r="C106" t="n">
-        <v/>
-      </c>
-      <c r="D106" t="n">
-        <v/>
-      </c>
-      <c r="E106" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>21-05-23 17:31:20</t>
-        </is>
-      </c>
-      <c r="B107" t="n">
-        <v/>
-      </c>
-      <c r="C107" t="n">
-        <v/>
-      </c>
-      <c r="D107" t="n">
-        <v/>
-      </c>
-      <c r="E107" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>21-05-23 17:31:22</t>
-        </is>
-      </c>
-      <c r="B108" t="n">
-        <v/>
-      </c>
-      <c r="C108" t="n">
-        <v/>
-      </c>
-      <c r="D108" t="n">
-        <v/>
-      </c>
-      <c r="E108" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>21-05-23 17:31:25</t>
-        </is>
-      </c>
-      <c r="B109" t="n">
-        <v/>
-      </c>
-      <c r="C109" t="n">
-        <v/>
-      </c>
-      <c r="D109" t="n">
-        <v/>
-      </c>
-      <c r="E109" t="n">
+      <c r="E71" t="n">
         <v/>
       </c>
     </row>

</xml_diff>